<commit_message>
Added 2way anova extended
</commit_message>
<xml_diff>
--- a/13C_Statistics_Summary.xlsx
+++ b/13C_Statistics_Summary.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTrevisan\Documents\GitHub\13C-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9090EC-8EBE-4ED9-8BF3-B9FC2B387879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E82B78-71AE-4A73-8399-89F7DC3C46A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoWayAnova" sheetId="1" r:id="rId1"/>
-    <sheet name="OneWayAnova_Tr" sheetId="2" r:id="rId2"/>
-    <sheet name="OneWayAnova_Ti" sheetId="3" r:id="rId3"/>
-    <sheet name="HSD_Tr" sheetId="5" r:id="rId4"/>
-    <sheet name="HSD_Ti" sheetId="6" r:id="rId5"/>
+    <sheet name="TwoWay Anova extended" sheetId="7" r:id="rId2"/>
+    <sheet name="OneWayAnova_Tr" sheetId="2" r:id="rId3"/>
+    <sheet name="OneWayAnova_Ti" sheetId="3" r:id="rId4"/>
+    <sheet name="HSD_Tr" sheetId="5" r:id="rId5"/>
+    <sheet name="HSD_Ti" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="211">
   <si>
     <t>Treatment</t>
   </si>
@@ -677,6 +678,9 @@
   </si>
   <si>
     <t>BS  --&gt; not to test (P=0.212)</t>
+  </si>
+  <si>
+    <t>&lt;2e-16</t>
   </si>
 </sst>
 </file>
@@ -745,7 +749,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -995,11 +999,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1033,6 +1072,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1474,6 +1517,1436 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8C5C5F-88C1-4356-B84D-2C2B3E287910}">
+  <dimension ref="A1:I96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>57.36</v>
+      </c>
+      <c r="D6">
+        <v>19.12</v>
+      </c>
+      <c r="E6">
+        <v>15.0482</v>
+      </c>
+      <c r="F6" s="23">
+        <v>1.0099999999999999E-8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1898.83</v>
+      </c>
+      <c r="D7">
+        <v>316.47000000000003</v>
+      </c>
+      <c r="E7">
+        <v>249.0839</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>22.04</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>0.96350000000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.50409999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>168</v>
+      </c>
+      <c r="C9">
+        <v>213.45</v>
+      </c>
+      <c r="D9">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>0.05</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>1.49</v>
+      </c>
+      <c r="D18">
+        <v>0.497</v>
+      </c>
+      <c r="E18">
+        <v>1.5154000000000001</v>
+      </c>
+      <c r="F18">
+        <v>0.21240000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>1513.14</v>
+      </c>
+      <c r="D19">
+        <v>252.19</v>
+      </c>
+      <c r="E19">
+        <v>768.39400000000001</v>
+      </c>
+      <c r="F19" t="s">
+        <v>210</v>
+      </c>
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>4.87</v>
+      </c>
+      <c r="D20">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="E20">
+        <v>0.82430000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.66990000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21">
+        <v>168</v>
+      </c>
+      <c r="C21">
+        <v>55.14</v>
+      </c>
+      <c r="D21">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23">
+        <v>1E-3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23">
+        <v>0.01</v>
+      </c>
+      <c r="H23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>0.05</v>
+      </c>
+      <c r="D24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24">
+        <v>0.1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>71.194000000000003</v>
+      </c>
+      <c r="D30">
+        <v>23.731200000000001</v>
+      </c>
+      <c r="E30">
+        <v>28.987200000000001</v>
+      </c>
+      <c r="F30" s="23">
+        <v>3.7199999999999997E-15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>115.901</v>
+      </c>
+      <c r="D31">
+        <v>19.316800000000001</v>
+      </c>
+      <c r="E31">
+        <v>23.595099999999999</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>18</v>
+      </c>
+      <c r="C32">
+        <v>81.42</v>
+      </c>
+      <c r="D32">
+        <v>4.5232999999999999</v>
+      </c>
+      <c r="E32">
+        <v>5.5251999999999999</v>
+      </c>
+      <c r="F32" s="23">
+        <v>4.3899999999999998E-10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33">
+        <v>168</v>
+      </c>
+      <c r="C33">
+        <v>137.53800000000001</v>
+      </c>
+      <c r="D33">
+        <v>0.81869999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35">
+        <v>1E-3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35">
+        <v>0.01</v>
+      </c>
+      <c r="H35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>0.05</v>
+      </c>
+      <c r="D36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36">
+        <v>0.1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" t="s">
+        <v>120</v>
+      </c>
+      <c r="H41" t="s">
+        <v>121</v>
+      </c>
+      <c r="I41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>56.137</v>
+      </c>
+      <c r="D42">
+        <v>18.712199999999999</v>
+      </c>
+      <c r="E42">
+        <v>38.128599999999999</v>
+      </c>
+      <c r="F42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>87.513000000000005</v>
+      </c>
+      <c r="D43">
+        <v>14.5855</v>
+      </c>
+      <c r="E43">
+        <v>29.719899999999999</v>
+      </c>
+      <c r="F43" t="s">
+        <v>139</v>
+      </c>
+      <c r="G43" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H43" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>18</v>
+      </c>
+      <c r="C44">
+        <v>60.947000000000003</v>
+      </c>
+      <c r="D44">
+        <v>3.3860000000000001</v>
+      </c>
+      <c r="E44">
+        <v>6.8994</v>
+      </c>
+      <c r="F44" s="23">
+        <v>7.3200000000000001E-13</v>
+      </c>
+      <c r="G44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45">
+        <v>168</v>
+      </c>
+      <c r="C45">
+        <v>82.448999999999998</v>
+      </c>
+      <c r="D45">
+        <v>0.49080000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47">
+        <v>1E-3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47">
+        <v>0.01</v>
+      </c>
+      <c r="H47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>0.05</v>
+      </c>
+      <c r="D48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48">
+        <v>0.1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" t="s">
+        <v>120</v>
+      </c>
+      <c r="H53" t="s">
+        <v>121</v>
+      </c>
+      <c r="I53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>0.8</v>
+      </c>
+      <c r="D54">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E54">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="F54">
+        <v>0.54269999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>334.36</v>
+      </c>
+      <c r="D55">
+        <v>55.725999999999999</v>
+      </c>
+      <c r="E55">
+        <v>149.1721</v>
+      </c>
+      <c r="F55" t="s">
+        <v>210</v>
+      </c>
+      <c r="G55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>18</v>
+      </c>
+      <c r="C56">
+        <v>8.65</v>
+      </c>
+      <c r="D56">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E56">
+        <v>1.2868999999999999</v>
+      </c>
+      <c r="F56">
+        <v>0.2019</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57">
+        <v>168</v>
+      </c>
+      <c r="C57">
+        <v>62.76</v>
+      </c>
+      <c r="D57">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59">
+        <v>1E-3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59">
+        <v>0.01</v>
+      </c>
+      <c r="H59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>0.05</v>
+      </c>
+      <c r="D60" t="s">
+        <v>131</v>
+      </c>
+      <c r="E60">
+        <v>0.1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>140</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" t="s">
+        <v>136</v>
+      </c>
+      <c r="E65" t="s">
+        <v>137</v>
+      </c>
+      <c r="F65" t="s">
+        <v>136</v>
+      </c>
+      <c r="G65" t="s">
+        <v>120</v>
+      </c>
+      <c r="H65" t="s">
+        <v>121</v>
+      </c>
+      <c r="I65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>21.28</v>
+      </c>
+      <c r="D66">
+        <v>7.0949999999999998</v>
+      </c>
+      <c r="E66">
+        <v>27.183800000000002</v>
+      </c>
+      <c r="F66" s="23">
+        <v>2.2099999999999999E-14</v>
+      </c>
+      <c r="G66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <v>363.1</v>
+      </c>
+      <c r="D67">
+        <v>60.515999999999998</v>
+      </c>
+      <c r="E67">
+        <v>231.87450000000001</v>
+      </c>
+      <c r="F67" t="s">
+        <v>139</v>
+      </c>
+      <c r="G67" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="D68">
+        <v>0.502</v>
+      </c>
+      <c r="E68">
+        <v>1.9216</v>
+      </c>
+      <c r="F68">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="G68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69">
+        <v>168</v>
+      </c>
+      <c r="C69">
+        <v>43.85</v>
+      </c>
+      <c r="D69">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>128</v>
+      </c>
+      <c r="E71">
+        <v>1E-3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>129</v>
+      </c>
+      <c r="G71">
+        <v>0.01</v>
+      </c>
+      <c r="H71" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>0.05</v>
+      </c>
+      <c r="D72" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72">
+        <v>0.1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>140</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D77" t="s">
+        <v>136</v>
+      </c>
+      <c r="E77" t="s">
+        <v>137</v>
+      </c>
+      <c r="F77" t="s">
+        <v>136</v>
+      </c>
+      <c r="G77" t="s">
+        <v>120</v>
+      </c>
+      <c r="H77" t="s">
+        <v>121</v>
+      </c>
+      <c r="I77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>75.989999999999995</v>
+      </c>
+      <c r="D78">
+        <v>25.331</v>
+      </c>
+      <c r="E78">
+        <v>61.479900000000001</v>
+      </c>
+      <c r="F78" t="s">
+        <v>139</v>
+      </c>
+      <c r="G78" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H78" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+      <c r="C79">
+        <v>521.25</v>
+      </c>
+      <c r="D79">
+        <v>86.876000000000005</v>
+      </c>
+      <c r="E79">
+        <v>210.8502</v>
+      </c>
+      <c r="F79" t="s">
+        <v>139</v>
+      </c>
+      <c r="G79" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <v>48.61</v>
+      </c>
+      <c r="D80">
+        <v>2.7</v>
+      </c>
+      <c r="E80">
+        <v>6.5538999999999996</v>
+      </c>
+      <c r="F80" s="23">
+        <v>3.5399999999999999E-12</v>
+      </c>
+      <c r="G80" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81">
+        <v>168</v>
+      </c>
+      <c r="C81">
+        <v>69.22</v>
+      </c>
+      <c r="D81">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>128</v>
+      </c>
+      <c r="E83">
+        <v>1E-3</v>
+      </c>
+      <c r="F83" t="s">
+        <v>129</v>
+      </c>
+      <c r="G83">
+        <v>0.01</v>
+      </c>
+      <c r="H83" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <v>0.05</v>
+      </c>
+      <c r="D84" t="s">
+        <v>131</v>
+      </c>
+      <c r="E84">
+        <v>0.1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>140</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" t="s">
+        <v>136</v>
+      </c>
+      <c r="E89" t="s">
+        <v>137</v>
+      </c>
+      <c r="F89" t="s">
+        <v>136</v>
+      </c>
+      <c r="G89" t="s">
+        <v>120</v>
+      </c>
+      <c r="H89" t="s">
+        <v>121</v>
+      </c>
+      <c r="I89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+      <c r="C90">
+        <v>53.155000000000001</v>
+      </c>
+      <c r="D90">
+        <v>17.718</v>
+      </c>
+      <c r="E90">
+        <v>47.802799999999998</v>
+      </c>
+      <c r="F90" t="s">
+        <v>139</v>
+      </c>
+      <c r="G90" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H90" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+      <c r="C91">
+        <v>194.53700000000001</v>
+      </c>
+      <c r="D91">
+        <v>32.423000000000002</v>
+      </c>
+      <c r="E91">
+        <v>87.474000000000004</v>
+      </c>
+      <c r="F91" t="s">
+        <v>139</v>
+      </c>
+      <c r="G91" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H91" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92">
+        <v>18</v>
+      </c>
+      <c r="C92">
+        <v>65.361000000000004</v>
+      </c>
+      <c r="D92">
+        <v>3.6309999999999998</v>
+      </c>
+      <c r="E92">
+        <v>9.7965999999999998</v>
+      </c>
+      <c r="F92" t="s">
+        <v>139</v>
+      </c>
+      <c r="G92" s="23">
+        <v>2.2E-16</v>
+      </c>
+      <c r="H92" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>124</v>
+      </c>
+      <c r="B93">
+        <v>168</v>
+      </c>
+      <c r="C93">
+        <v>62.27</v>
+      </c>
+      <c r="D93">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" t="s">
+        <v>127</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
+        <v>128</v>
+      </c>
+      <c r="E95">
+        <v>1E-3</v>
+      </c>
+      <c r="F95" t="s">
+        <v>129</v>
+      </c>
+      <c r="G95">
+        <v>0.01</v>
+      </c>
+      <c r="H95" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C96">
+        <v>0.05</v>
+      </c>
+      <c r="D96" t="s">
+        <v>131</v>
+      </c>
+      <c r="E96">
+        <v>0.1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>140</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2E0E9C-5AC7-4095-B085-BD64FFD9B693}">
   <dimension ref="A1:H518"/>
   <sheetViews>
@@ -7496,7 +8969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37239465-76AF-4EE1-8B0F-9533E7F5CF30}">
   <dimension ref="A1:H329"/>
   <sheetViews>
@@ -11377,15 +12850,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FB93C6-0778-4F99-B1A3-133ED5E9BF6D}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11426,7 +12899,7 @@
       <c r="G2" s="13">
         <v>11</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="33">
         <v>14</v>
       </c>
     </row>
@@ -11452,7 +12925,7 @@
       <c r="G3" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="34" t="s">
         <v>166</v>
       </c>
     </row>
@@ -11478,7 +12951,7 @@
       <c r="G4" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="35" t="s">
         <v>90</v>
       </c>
     </row>
@@ -11504,7 +12977,7 @@
       <c r="G5" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="35" t="s">
         <v>108</v>
       </c>
     </row>
@@ -11530,7 +13003,7 @@
       <c r="G6" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -11556,7 +13029,7 @@
       <c r="G7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="36" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11590,7 +13063,7 @@
       <c r="G10" s="13">
         <v>11</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="33">
         <v>14</v>
       </c>
     </row>
@@ -11616,7 +13089,7 @@
       <c r="G11" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="34" t="s">
         <v>166</v>
       </c>
     </row>
@@ -11642,7 +13115,7 @@
       <c r="G12" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11668,7 +13141,7 @@
       <c r="G13" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11694,7 +13167,7 @@
       <c r="G14" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -11720,7 +13193,7 @@
       <c r="G15" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="36" t="s">
         <v>85</v>
       </c>
     </row>
@@ -11754,7 +13227,7 @@
       <c r="G18" s="13">
         <v>12</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="33">
         <v>14</v>
       </c>
     </row>
@@ -11780,7 +13253,7 @@
       <c r="G19" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="34" t="s">
         <v>166</v>
       </c>
     </row>
@@ -11806,7 +13279,7 @@
       <c r="G20" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11832,7 +13305,7 @@
       <c r="G21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11858,7 +13331,7 @@
       <c r="G22" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -11884,7 +13357,7 @@
       <c r="G23" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="36" t="s">
         <v>85</v>
       </c>
     </row>
@@ -11918,7 +13391,7 @@
       <c r="G26" s="13">
         <v>12</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="33">
         <v>14</v>
       </c>
     </row>
@@ -11944,7 +13417,7 @@
       <c r="G27" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="34" t="s">
         <v>166</v>
       </c>
     </row>
@@ -11970,7 +13443,7 @@
       <c r="G28" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11996,7 +13469,7 @@
       <c r="G29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12022,7 +13495,7 @@
       <c r="G30" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12048,7 +13521,7 @@
       <c r="G31" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="36" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12082,7 +13555,7 @@
       <c r="G34" s="13">
         <v>11</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H34" s="33">
         <v>14</v>
       </c>
     </row>
@@ -12108,7 +13581,7 @@
       <c r="G35" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="34" t="s">
         <v>168</v>
       </c>
     </row>
@@ -12134,7 +13607,7 @@
       <c r="G36" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12160,7 +13633,7 @@
       <c r="G37" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H37" s="35" t="s">
         <v>105</v>
       </c>
     </row>
@@ -12186,7 +13659,7 @@
       <c r="G38" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="H38" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12212,7 +13685,7 @@
       <c r="G39" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="36" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12246,7 +13719,7 @@
       <c r="G42" s="13">
         <v>11</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H42" s="33">
         <v>14</v>
       </c>
     </row>
@@ -12272,7 +13745,7 @@
       <c r="G43" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H43" s="10" t="s">
+      <c r="H43" s="34" t="s">
         <v>166</v>
       </c>
     </row>
@@ -12298,7 +13771,7 @@
       <c r="G44" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H44" s="15" t="s">
+      <c r="H44" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12324,7 +13797,7 @@
       <c r="G45" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="H45" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12350,7 +13823,7 @@
       <c r="G46" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="H46" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12376,7 +13849,7 @@
       <c r="G47" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="36" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12410,7 +13883,7 @@
       <c r="G50" s="13">
         <v>11</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H50" s="33">
         <v>14</v>
       </c>
     </row>
@@ -12436,7 +13909,7 @@
       <c r="G51" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H51" s="34" t="s">
         <v>171</v>
       </c>
     </row>
@@ -12462,7 +13935,7 @@
       <c r="G52" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="H52" s="15" t="s">
+      <c r="H52" s="35" t="s">
         <v>105</v>
       </c>
     </row>
@@ -12488,7 +13961,7 @@
       <c r="G53" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="H53" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12514,7 +13987,7 @@
       <c r="G54" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H54" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12540,7 +14013,7 @@
       <c r="G55" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H55" s="20" t="s">
+      <c r="H55" s="36" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12574,7 +14047,7 @@
       <c r="G58" s="13">
         <v>11</v>
       </c>
-      <c r="H58" s="13">
+      <c r="H58" s="33">
         <v>14</v>
       </c>
     </row>
@@ -12600,7 +14073,7 @@
       <c r="G59" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="H59" s="34" t="s">
         <v>208</v>
       </c>
     </row>
@@ -12626,7 +14099,7 @@
       <c r="G60" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H60" s="15" t="s">
+      <c r="H60" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12652,7 +14125,7 @@
       <c r="G61" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H61" s="15" t="s">
+      <c r="H61" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12678,7 +14151,7 @@
       <c r="G62" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H62" s="15" t="s">
+      <c r="H62" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12704,7 +14177,7 @@
       <c r="G63" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="H63" s="20" t="s">
+      <c r="H63" s="36" t="s">
         <v>85</v>
       </c>
     </row>
@@ -12731,14 +14204,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0067E492-B4A5-4E75-AECD-DA5DE7917A5A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>